<commit_message>
MPSTOOLS-1 - Finished Quotegen Models
</commit_message>
<xml_diff>
--- a/public/downloads/order-list.xlsx
+++ b/public/downloads/order-list.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>Hardware Device List</t>
   </si>
@@ -38,28 +38,22 @@
     <t>Location</t>
   </si>
   <si>
-    <t>HP Color LaserJet CM6040f</t>
-  </si>
-  <si>
-    <t>Q3939A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     HP Booklet Maker/Finisher with Output</t>
-  </si>
-  <si>
-    <t>CC516A</t>
-  </si>
-  <si>
-    <t>Device 2</t>
-  </si>
-  <si>
-    <t>Device 3</t>
-  </si>
-  <si>
-    <t>Device 4</t>
-  </si>
-  <si>
-    <t>Device 5</t>
+    <t>HP LaserJet M9050</t>
+  </si>
+  <si>
+    <t>CC395A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     8-Bin Mailbox</t>
+  </si>
+  <si>
+    <t>Q5693A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     HP LaserJet MFP 3000-sheet Stapler/Stacker</t>
+  </si>
+  <si>
+    <t>C8085A</t>
   </si>
 </sst>
 </file>
@@ -431,10 +425,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -498,169 +492,20 @@
       </c>
       <c r="C6"/>
     </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="2" t="s">
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="2" t="s">
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24"/>
+      <c r="C7"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A8:E8"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A21:E21"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>